<commit_message>
add Homework Week 1
</commit_message>
<xml_diff>
--- a/Week 1/Class_2_Activities/04-Stu_GradeBook/Unsolved/GradeBook_Unsolved.xlsx
+++ b/Week 1/Class_2_Activities/04-Stu_GradeBook/Unsolved/GradeBook_Unsolved.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dcorless/Documents/coding-boot-camp/DataViz-Lesson-Plans/01-Lesson-Plans/01-Excel/2/Activities/04-Stu_GradeBook/Unsolved/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anja/UCB_Course/UCB-data-course/Week 1/Class_2_Activities/04-Stu_GradeBook/Unsolved/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF38C4B4-A970-E24A-88BC-430FC4505103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84219B14-CD5F-1942-8EC2-67DE8679EC8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="20500" windowHeight="13100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="24780" windowHeight="13100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -194,11 +194,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -519,7 +519,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="B2:E25"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -556,436 +556,508 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>60</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>93</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>71</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <v>73</v>
       </c>
-      <c r="F2" s="2"/>
+      <c r="F2" s="4">
+        <f>AVERAGE(B2:E2)</f>
+        <v>74.25</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>93</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>73</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>82</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>75</v>
       </c>
-      <c r="F3" s="2"/>
+      <c r="F3" s="4">
+        <f t="shared" ref="F3:F25" si="0">AVERAGE(B3:E3)</f>
+        <v>80.75</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>60</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>79</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>75</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>97</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="4">
+        <f t="shared" si="0"/>
+        <v>77.75</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>63</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>58</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>82</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>49</v>
       </c>
-      <c r="F5" s="2"/>
+      <c r="F5" s="4">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>59</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>91</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>64</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>56</v>
       </c>
-      <c r="F6" s="2"/>
+      <c r="F6" s="4">
+        <f t="shared" si="0"/>
+        <v>67.5</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>43</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>42</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>95</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>50</v>
       </c>
-      <c r="F7" s="2"/>
+      <c r="F7" s="4">
+        <f t="shared" si="0"/>
+        <v>57.5</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>81</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>96</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>42</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>68</v>
       </c>
-      <c r="F8" s="2"/>
+      <c r="F8" s="4">
+        <f t="shared" si="0"/>
+        <v>71.75</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>100</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>95</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>94</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>89</v>
       </c>
-      <c r="F9" s="2"/>
+      <c r="F9" s="4">
+        <f t="shared" si="0"/>
+        <v>94.5</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <v>89</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>92</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>71</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>93</v>
       </c>
-      <c r="F10" s="2"/>
+      <c r="F10" s="4">
+        <f t="shared" si="0"/>
+        <v>86.25</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="3">
         <v>55</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <v>83</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <v>79</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <v>45</v>
       </c>
-      <c r="F11" s="2"/>
+      <c r="F11" s="4">
+        <f t="shared" si="0"/>
+        <v>65.5</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="3">
         <v>58</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="3">
         <v>93</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3">
         <v>57</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="3">
         <v>94</v>
       </c>
-      <c r="F12" s="2"/>
+      <c r="F12" s="4">
+        <f t="shared" si="0"/>
+        <v>75.5</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="3">
         <v>53</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="3">
         <v>49</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="3">
         <v>94</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="3">
         <v>87</v>
       </c>
-      <c r="F13" s="2"/>
+      <c r="F13" s="4">
+        <f t="shared" si="0"/>
+        <v>70.75</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="3">
         <v>89</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="3">
         <v>88</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="3">
         <v>69</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="3">
         <v>98</v>
       </c>
-      <c r="F14" s="2"/>
+      <c r="F14" s="4">
+        <f t="shared" si="0"/>
+        <v>86</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="3">
         <v>46</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="3">
         <v>48</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="3">
         <v>94</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="3">
         <v>91</v>
       </c>
-      <c r="F15" s="2"/>
+      <c r="F15" s="4">
+        <f t="shared" si="0"/>
+        <v>69.75</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="3">
         <v>99</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="3">
         <v>81</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="3">
         <v>51</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="3">
         <v>91</v>
       </c>
-      <c r="F16" s="2"/>
+      <c r="F16" s="4">
+        <f t="shared" si="0"/>
+        <v>80.5</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="3">
         <v>96</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="3">
         <v>83</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="3">
         <v>99</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="3">
         <v>93</v>
       </c>
-      <c r="F17" s="2"/>
+      <c r="F17" s="4">
+        <f t="shared" si="0"/>
+        <v>92.75</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="3">
         <v>44</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="3">
         <v>59</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="3">
         <v>61</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="3">
         <v>48</v>
       </c>
-      <c r="F18" s="2"/>
+      <c r="F18" s="4">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19" s="3">
         <v>50</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="3">
         <v>80</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D19" s="3">
         <v>84</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="3">
         <v>96</v>
       </c>
-      <c r="F19" s="2"/>
+      <c r="F19" s="4">
+        <f t="shared" si="0"/>
+        <v>77.5</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="3">
         <v>49</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="3">
         <v>77</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D20" s="3">
         <v>62</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="3">
         <v>84</v>
       </c>
-      <c r="F20" s="2"/>
+      <c r="F20" s="4">
+        <f t="shared" si="0"/>
+        <v>68</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21" s="3">
         <v>45</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="3">
         <v>83</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D21" s="3">
         <v>70</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="3">
         <v>65</v>
       </c>
-      <c r="F21" s="2"/>
+      <c r="F21" s="4">
+        <f t="shared" si="0"/>
+        <v>65.75</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22" s="3">
         <v>43</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="3">
         <v>62</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D22" s="3">
         <v>60</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E22" s="3">
         <v>71</v>
       </c>
-      <c r="F22" s="2"/>
+      <c r="F22" s="4">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23" s="3">
         <v>54</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23" s="3">
         <v>50</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D23" s="3">
         <v>92</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23" s="3">
         <v>52</v>
       </c>
-      <c r="F23" s="2"/>
+      <c r="F23" s="4">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B24" s="3">
         <v>96</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="3">
         <v>96</v>
       </c>
-      <c r="D24" s="4">
+      <c r="D24" s="3">
         <v>70</v>
       </c>
-      <c r="E24" s="4">
+      <c r="E24" s="3">
         <v>98</v>
       </c>
-      <c r="F24" s="2"/>
+      <c r="F24" s="4">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25" s="3">
         <v>59</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25" s="3">
         <v>66</v>
       </c>
-      <c r="D25" s="4">
+      <c r="D25" s="3">
         <v>49</v>
       </c>
-      <c r="E25" s="4">
+      <c r="E25" s="3">
         <v>98</v>
       </c>
-      <c r="F25" s="2"/>
+      <c r="F25" s="4">
+        <f t="shared" si="0"/>
+        <v>68</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>